<commit_message>
Automation-Positive Flow with Report
</commit_message>
<xml_diff>
--- a/ECommerceDemo/src/test/resources/testData/Data.xlsx
+++ b/ECommerceDemo/src/test/resources/testData/Data.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19488" windowHeight="3396" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9144" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
     <sheet name="ProductData" sheetId="2" r:id="rId2"/>
-    <sheet name="OrderData" sheetId="3" r:id="rId3"/>
+    <sheet name="OrderFormData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:B2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -31,7 +30,7 @@
     <t>Iamking@000</t>
   </si>
   <si>
-    <t>ProductName</t>
+    <t>ProductName1</t>
   </si>
   <si>
     <r>
@@ -45,33 +44,124 @@
     </r>
   </si>
   <si>
-    <t>ProductPrice</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF6C757D"/>
-        <rFont val="Segoe UI"/>
-        <charset val="134"/>
-      </rPr>
-      <t>$ 31500</t>
-    </r>
-  </si>
-  <si>
-    <t>OrderId</t>
+    <t>ProductPrice1</t>
+  </si>
+  <si>
+    <t>31500</t>
+  </si>
+  <si>
+    <t>ProductName2</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="9.95"/>
         <color rgb="FF212529"/>
         <rFont val="Segoe UI"/>
         <charset val="134"/>
       </rPr>
-      <t>65dec1caa86f8f74dc8a1bbc</t>
+      <t>ADIDAS ORIGINAL</t>
     </r>
+  </si>
+  <si>
+    <t>ProductPrice2</t>
+  </si>
+  <si>
+    <t>ProductName3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.95"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>IPHONE 13 PRO</t>
+    </r>
+  </si>
+  <si>
+    <t>ProductPrice3</t>
+  </si>
+  <si>
+    <t>ProductName4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.95"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ABCD</t>
+    </r>
+  </si>
+  <si>
+    <t>ProductPrice4</t>
+  </si>
+  <si>
+    <t>ProductName5</t>
+  </si>
+  <si>
+    <t>ProductPrice5</t>
+  </si>
+  <si>
+    <t>ProductName6</t>
+  </si>
+  <si>
+    <t>ProductPrice6</t>
+  </si>
+  <si>
+    <t>ProductName7</t>
+  </si>
+  <si>
+    <t>ProductPrice7</t>
+  </si>
+  <si>
+    <t>ProductName8</t>
+  </si>
+  <si>
+    <t>ProductPrice8</t>
+  </si>
+  <si>
+    <t>ProductName9</t>
+  </si>
+  <si>
+    <t>ProductPrice9</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Credit Card Number</t>
+  </si>
+  <si>
+    <t>4542 9931 9292 2293</t>
+  </si>
+  <si>
+    <t>cvv</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>nandhana</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>65e1be0ea86f8f74dc8d03ff</t>
   </si>
 </sst>
 </file>
@@ -84,7 +174,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,10 +183,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
+      <sz val="10.5"/>
+      <color rgb="FF616161"/>
+      <name val="Helvetica"/>
       <charset val="134"/>
     </font>
     <font>
@@ -108,6 +197,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF6C757D"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.95"/>
+      <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
@@ -584,150 +680,159 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1264,7 +1369,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1277,7 +1382,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1285,7 +1390,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1302,15 +1407,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="18.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="11.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1318,7 +1423,7 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1326,8 +1431,136 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="1:2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="19.2" spans="1:2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <v>31500</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="19.2" spans="1:2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>231500</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="19.2" spans="1:2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="19.2" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" ht="19.2" spans="1:2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" ht="19.2" spans="1:2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" ht="19.2" spans="1:2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="19.2" spans="1:2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="6">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -1339,23 +1572,55 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="2" max="2" width="34.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.2" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Positive Flow with report
</commit_message>
<xml_diff>
--- a/ECommerceDemo/src/test/resources/testData/Data.xlsx
+++ b/ECommerceDemo/src/test/resources/testData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" activeTab="1"/>
+    <workbookView windowWidth="17448" windowHeight="7727"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="OrderFormData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:B18"/>
 </workbook>
 </file>
 
@@ -1368,7 +1369,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1409,7 +1410,7 @@
   <sheetPr/>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>